<commit_message>
Add transcriptomics to template and schema for experiment type
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2278001B-B920-8843-AD00-DFD8CF38C27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ED1E1F-6A6B-AC46-A201-0ACACB7B5D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="559">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -1853,6 +1853,9 @@
   </si>
   <si>
     <t>restricted access</t>
+  </si>
+  <si>
+    <t>transcriptomics</t>
   </si>
 </sst>
 </file>
@@ -2263,44 +2266,14 @@
   </cellStyleXfs>
   <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2310,9 +2283,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2408,6 +2378,39 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2820,209 +2823,214 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="29" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
     <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="65"/>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="320" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="60"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="60"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="60"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
+      <c r="B22" s="60"/>
+    </row>
+    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3032,11 +3040,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3060,16 +3063,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="18" t="s">
         <v>259</v>
       </c>
     </row>
@@ -3117,7 +3120,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G281"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3128,34 +3133,34 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="58" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="58" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="23" t="s">
         <v>79</v>
       </c>
       <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="23" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3172,7 +3177,7 @@
       <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="59"/>
       <c r="G3" t="s">
         <v>261</v>
       </c>
@@ -3271,6 +3276,9 @@
       <c r="B10" t="s">
         <v>284</v>
       </c>
+      <c r="D10" t="s">
+        <v>558</v>
+      </c>
       <c r="E10" t="s">
         <v>109</v>
       </c>
@@ -3626,7 +3634,7 @@
       <c r="B54" t="s">
         <v>330</v>
       </c>
-      <c r="E54" s="46"/>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
@@ -4764,7 +4772,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6IlNjdvVsk0k7AI4npJ2J9WUgUSdSMaDFjio234Tp28J/obtzzDxUQwtc4aqsO7xgbOXLFGVCIW4c6yTV1DUNQ==" saltValue="tkrgJBF4YSc+55smwh3JLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZaCRVRElACVekRp0xmCPvUwZWwwkmCSdRJFCsYkHVAWOLYAM+2KQYAc46a1lkDzs3xaJUYYA7iFOMEtYTV/SzQ==" saltValue="sVc+BDvgYCKBXWavk4P37g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4790,25 +4798,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4822,7 +4830,7 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="20" t="s">
         <v>33</v>
       </c>
       <c r="E2" t="s">
@@ -4845,13 +4853,13 @@
       <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
@@ -4883,15 +4891,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
@@ -4899,7 +4907,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
@@ -4907,7 +4915,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
@@ -4915,15 +4923,15 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B6" t="s">
@@ -5003,10 +5011,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="25" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5037,61 +5045,61 @@
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="40.5" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="37" customWidth="1"/>
+    <col min="11" max="11" width="16.5" style="26" customWidth="1"/>
     <col min="12" max="12" width="64.83203125" customWidth="1"/>
     <col min="13" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="29" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J2" s="12"/>
+      <c r="J2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5113,7 +5121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5122,15 +5132,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
       <c r="B2" t="s">
@@ -5138,7 +5148,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B3" t="s">
@@ -5146,7 +5156,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
@@ -5154,7 +5164,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
@@ -5162,7 +5172,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="23" t="s">
         <v>79</v>
       </c>
       <c r="B6" t="s">
@@ -5170,7 +5180,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="23" t="s">
         <v>81</v>
       </c>
       <c r="B7" t="s">
@@ -5250,7 +5260,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="23" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5542,58 +5552,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="27" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="36"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="36"/>
+      <c r="C4" s="25"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5659,68 +5669,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="31" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="32" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="31" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="31" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="34" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="31" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -5728,7 +5738,7 @@
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="31" t="s">
         <v>165</v>
       </c>
     </row>
@@ -5736,7 +5746,7 @@
       <c r="A11" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="31" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5744,7 +5754,7 @@
       <c r="A12" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="31" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5752,29 +5762,29 @@
       <c r="A13" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="31" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="42"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="36" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="31" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5782,21 +5792,21 @@
       <c r="A17" t="s">
         <v>177</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="31" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>180</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="31" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5804,21 +5814,21 @@
       <c r="A20" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="31" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="42"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="31" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5826,7 +5836,7 @@
       <c r="A23" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="31" t="s">
         <v>188</v>
       </c>
     </row>
@@ -5834,7 +5844,7 @@
       <c r="A24" t="s">
         <v>189</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="31" t="s">
         <v>190</v>
       </c>
     </row>
@@ -5842,7 +5852,7 @@
       <c r="A25" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="31" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5850,21 +5860,21 @@
       <c r="A26" t="s">
         <v>193</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="42"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="31" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5872,7 +5882,7 @@
       <c r="A29" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="31" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5880,21 +5890,21 @@
       <c r="A30" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="31" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B31" s="42"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>203</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="31" t="s">
         <v>204</v>
       </c>
     </row>
@@ -5902,7 +5912,7 @@
       <c r="A33" t="s">
         <v>205</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="31" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5910,7 +5920,7 @@
       <c r="A34" t="s">
         <v>207</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="31" t="s">
         <v>208</v>
       </c>
     </row>
@@ -5918,7 +5928,7 @@
       <c r="A35" t="s">
         <v>209</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="31" t="s">
         <v>210</v>
       </c>
     </row>
@@ -5926,7 +5936,7 @@
       <c r="A36" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="31" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5934,7 +5944,7 @@
       <c r="A37" t="s">
         <v>213</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="31" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5942,7 +5952,7 @@
       <c r="A38" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="31" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5950,7 +5960,7 @@
       <c r="A39" t="s">
         <v>217</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="31" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5958,7 +5968,7 @@
       <c r="A40" t="s">
         <v>219</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="31" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5966,21 +5976,21 @@
       <c r="A41" t="s">
         <v>221</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="36" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="B42" s="42"/>
+      <c r="B42" s="31"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>224</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="31" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5988,7 +5998,7 @@
       <c r="A44" t="s">
         <v>226</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="31" t="s">
         <v>227</v>
       </c>
     </row>
@@ -5996,7 +6006,7 @@
       <c r="A45" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="31" t="s">
         <v>229</v>
       </c>
     </row>
@@ -6004,7 +6014,7 @@
       <c r="A46" t="s">
         <v>230</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="31" t="s">
         <v>231</v>
       </c>
     </row>
@@ -6012,7 +6022,7 @@
       <c r="A47" t="s">
         <v>232</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="31" t="s">
         <v>233</v>
       </c>
     </row>
@@ -6020,7 +6030,7 @@
       <c r="A48" t="s">
         <v>234</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="31" t="s">
         <v>235</v>
       </c>
     </row>
@@ -6028,7 +6038,7 @@
       <c r="A49" t="s">
         <v>236</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="31" t="s">
         <v>237</v>
       </c>
     </row>
@@ -6036,7 +6046,7 @@
       <c r="A50" t="s">
         <v>238</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="31" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6044,7 +6054,7 @@
       <c r="A51" t="s">
         <v>240</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="31" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6052,33 +6062,33 @@
       <c r="A52" t="s">
         <v>242</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="31" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="B53" s="42"/>
+      <c r="B53" s="31"/>
     </row>
     <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="B54" s="42"/>
+      <c r="B54" s="31"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="48" t="s">
+      <c r="A55" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="B55" s="42"/>
+      <c r="B55" s="31"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>247</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="31" t="s">
         <v>248</v>
       </c>
     </row>
@@ -6106,262 +6116,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A1" s="49"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="55"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="42"/>
+      <c r="AL1" s="42"/>
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="42"/>
+      <c r="AP1" s="42"/>
+      <c r="AQ1" s="42"/>
+      <c r="AR1" s="44"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="1" t="s">
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="70" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="2" t="s">
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="68" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2" t="s">
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2" t="s">
+      <c r="Y2" s="68"/>
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="68"/>
+      <c r="AB2" s="68"/>
+      <c r="AC2" s="68"/>
+      <c r="AD2" s="68"/>
+      <c r="AE2" s="68"/>
+      <c r="AF2" s="68"/>
+      <c r="AG2" s="68"/>
+      <c r="AH2" s="68" t="s">
         <v>223</v>
       </c>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
+      <c r="AI2" s="68"/>
+      <c r="AJ2" s="68"/>
+      <c r="AK2" s="68"/>
+      <c r="AL2" s="68"/>
+      <c r="AM2" s="68"/>
+      <c r="AN2" s="68"/>
+      <c r="AO2" s="68"/>
+      <c r="AP2" s="68"/>
+      <c r="AQ2" s="68"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="L3" s="63" t="s">
+      <c r="L3" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="O3" s="62" t="s">
+      <c r="O3" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="P3" s="65" t="s">
+      <c r="P3" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="Q3" s="62" t="s">
+      <c r="Q3" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="R3" s="62" t="s">
+      <c r="R3" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="S3" s="62" t="s">
+      <c r="S3" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="T3" s="63" t="s">
+      <c r="T3" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="U3" s="65" t="s">
+      <c r="U3" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="V3" s="62" t="s">
+      <c r="V3" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="W3" s="63" t="s">
+      <c r="W3" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="X3" s="65" t="s">
+      <c r="X3" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="Y3" s="66" t="s">
+      <c r="Y3" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="Z3" s="62" t="s">
+      <c r="Z3" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="AA3" s="62" t="s">
+      <c r="AA3" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="AB3" s="62" t="s">
+      <c r="AB3" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="AC3" s="62" t="s">
+      <c r="AC3" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="AD3" s="62" t="s">
+      <c r="AD3" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="AE3" s="62" t="s">
+      <c r="AE3" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="AF3" s="62" t="s">
+      <c r="AF3" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="AG3" s="63" t="s">
+      <c r="AG3" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="AH3" s="65" t="s">
+      <c r="AH3" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="AI3" s="62" t="s">
+      <c r="AI3" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="AJ3" s="62" t="s">
+      <c r="AJ3" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="AK3" s="62" t="s">
+      <c r="AK3" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="AL3" s="62" t="s">
+      <c r="AL3" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="AM3" s="62" t="s">
+      <c r="AM3" s="51" t="s">
         <v>234</v>
       </c>
-      <c r="AN3" s="62" t="s">
+      <c r="AN3" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="AO3" s="62" t="s">
+      <c r="AO3" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="AP3" s="62" t="s">
+      <c r="AP3" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="AQ3" s="63" t="s">
+      <c r="AQ3" s="52" t="s">
         <v>242</v>
       </c>
-      <c r="AR3" s="67" t="s">
+      <c r="AR3" s="56" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="K4" s="68"/>
-      <c r="W4" s="37"/>
+      <c r="K4" s="57"/>
+      <c r="W4" s="26"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="K5" s="68"/>
-      <c r="W5" s="37"/>
+      <c r="K5" s="57"/>
+      <c r="W5" s="26"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="K6" s="68"/>
-      <c r="W6" s="37"/>
+      <c r="K6" s="57"/>
+      <c r="W6" s="26"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="K7" s="68"/>
+      <c r="K7" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6439,15 +6449,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B2" t="s">
@@ -6455,7 +6465,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="23" t="s">
         <v>255</v>
       </c>
       <c r="B3" t="s">
@@ -6463,7 +6473,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="23" t="s">
         <v>257</v>
       </c>
       <c r="B4" t="s">
@@ -6471,7 +6481,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="23" t="s">
         <v>259</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
Remove Telephone number, Project alias, Project title from analysis, MD5 from files
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C60809-ACD5-A343-8F9A-16ED43CB88E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A758F62-72E6-D546-83C1-149F9777A6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="539">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Projects consist of analyses that are run on samples. We accept sample information in the form of BioSample, ENA or EGA accession(s). We also accept BioSamples sampleset accessions. If your samples are not yet accessioned, and are therefore novel, please use the "Novel sample(s)" sections of the Sample(s) worksheet to have them registered at BioSamples.</t>
-  </si>
-  <si>
     <t>Analysis</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Telephone Number</t>
-  </si>
-  <si>
     <t>Email Address</t>
   </si>
   <si>
@@ -153,12 +147,6 @@
     <t>Title of the project</t>
   </si>
   <si>
-    <t>Project Alias</t>
-  </si>
-  <si>
-    <t>Shortened identifier for the project</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -252,9 +240,6 @@
     <t>Description of the analysis</t>
   </si>
   <si>
-    <t>Title of the project to which this analysis belongs</t>
-  </si>
-  <si>
     <t>Experiment Type</t>
   </si>
   <si>
@@ -789,21 +774,6 @@
     <t>File name</t>
   </si>
   <si>
-    <t>File Type</t>
-  </si>
-  <si>
-    <t>File type from the following "vcf" &amp; "tabix"</t>
-  </si>
-  <si>
-    <t>MD5</t>
-  </si>
-  <si>
-    <t>MD5 value of the file - if you are unsure of this, please leave this blank</t>
-  </si>
-  <si>
-    <t>vcf</t>
-  </si>
-  <si>
     <t>Sample(s)</t>
   </si>
   <si>
@@ -819,9 +789,6 @@
     <t>Whole transcriptome sequencing</t>
   </si>
   <si>
-    <t>tabix</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -1693,9 +1660,6 @@
   </si>
   <si>
     <t>OR</t>
-  </si>
-  <si>
-    <t>V1.1.6 March 2024</t>
   </si>
   <si>
     <r>
@@ -1817,6 +1781,15 @@
       <t xml:space="preserve"> requirement.</t>
     </r>
   </si>
+  <si>
+    <t>V1.1.6 May 2024</t>
+  </si>
+  <si>
+    <t>This Spreadsheet is meant to be used with the EVA submissions command line tools eva-sub-cli.</t>
+  </si>
+  <si>
+    <t>Projects consist of analyses that are run on samples. We accept sample information in the form of BioSample accession(s). If your samples are not yet accessioned, and are therefore novel, please use the "Novel sample(s)" sections of the Sample(s) worksheet to have them registered at BioSamples.</t>
+  </si>
 </sst>
 </file>
 
@@ -1825,7 +1798,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2009,6 +1982,19 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2237,7 +2223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2340,6 +2326,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2358,45 +2367,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2806,7 +2798,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2817,8 +2809,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2827,10 +2819,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -2839,10 +2831,10 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
-        <v>546</v>
-      </c>
-      <c r="B3" s="61"/>
+      <c r="A3" s="70" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="70"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -2851,10 +2843,10 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="57"/>
+      <c r="A4" s="71" t="s">
+        <v>537</v>
+      </c>
+      <c r="B4" s="71"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2862,9 +2854,11 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="72"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2885,10 +2879,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -2897,8 +2891,8 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2907,10 +2901,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="57"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2919,8 +2913,8 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2929,12 +2923,12 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="59"/>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="B11" s="68"/>
+    </row>
+    <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
@@ -2959,60 +2953,60 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="100" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>13</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="100" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="64" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="76" t="s">
+      <c r="B19" s="64"/>
+    </row>
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="64" t="s">
+        <v>535</v>
+      </c>
+      <c r="B20" s="64"/>
+    </row>
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="76"/>
-    </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="76" t="s">
-        <v>547</v>
-      </c>
-      <c r="B20" s="76"/>
-    </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="76" t="s">
+      <c r="B21" s="64"/>
+    </row>
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="76"/>
-    </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="76" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="64"/>
     </row>
     <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0H1OqsSda8KaSyTd91X5XgzkJbaiqKu/QOiMrnZ6li9ATLrZtGNKDN9LnJsmRANQJtNNaAnlZxfj+Avw12WKXg==" saltValue="tQ94nNFt17NHC+1AeL/QdQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="MU1Ou8RkXCF2skpaTyap/rRlZ+lXNAvg7/CyPYvfUYxtHCfavXm69adfvvk8zyvIy5h/lXQdbiRBEwTzoTRiLA==" saltValue="3N3jbQAkrMCjyhvDt9mNXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -3035,40 +3029,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="VCF &amp; index" prompt="vcf or tabix" sqref="C1" xr:uid="{00000000-0002-0000-0900-000000000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -3078,7 +3060,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" xr:uid="{00000000-0002-0000-0900-000002000000}">
           <x14:formula1>
             <xm:f>Analysis!$B$2:$B$1000000</xm:f>
@@ -3088,15 +3070,6 @@
           </x14:formula2>
           <xm:sqref>A2:A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="File type does not equal vcf or tabix" xr:uid="{00000000-0002-0000-0900-000003000000}">
-          <x14:formula1>
-            <xm:f>CVs!$G$3:$G$4</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C2:C1004</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3105,9 +3078,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G281"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3115,1646 +3090,1633 @@
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="55"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="54" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D4" t="s">
-        <v>253</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" t="s">
         <v>90</v>
       </c>
-      <c r="G4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>258</v>
-      </c>
-      <c r="B6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D6" t="s">
-        <v>260</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>261</v>
+      </c>
+      <c r="B11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B7" t="s">
-        <v>262</v>
-      </c>
-      <c r="D7" t="s">
-        <v>263</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>264</v>
-      </c>
-      <c r="B8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>266</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>267</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>268</v>
       </c>
-      <c r="D9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>270</v>
-      </c>
-      <c r="B10" t="s">
-        <v>271</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E16" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" t="s">
-        <v>273</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B12" t="s">
-        <v>275</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>276</v>
-      </c>
-      <c r="E13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>277</v>
-      </c>
-      <c r="E14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>278</v>
-      </c>
-      <c r="E15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>279</v>
-      </c>
-      <c r="E16" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="E30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="E40" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="E43" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E46" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="E47" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="E49" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E50" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="E51" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E54" s="36"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6IlNjdvVsk0k7AI4npJ2J9WUgUSdSMaDFjio234Tp28J/obtzzDxUQwtc4aqsO7xgbOXLFGVCIW4c6yTV1DUNQ==" saltValue="tkrgJBF4YSc+55smwh3JLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YpxYS3YarbEcU6tWwuRMfCKS/4VgrVauR8PgXRA9n+H1kMj1rZpzdUBeRpn2V18P1MjYz2grSS8/2LmiS55opA==" saltValue="fjdpxiVJrkefuObTwVSAQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4762,52 +4724,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" customWidth="1"/>
-    <col min="7" max="7" width="51" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.25">
-      <c r="D3" s="21"/>
-      <c r="F3" s="22"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C3" s="21"/>
+      <c r="E3" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4817,10 +4775,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4831,134 +4789,126 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="B6" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="STzJTlcpWbMUCdd3KhVcmCxC2DwAFiSWwnxUq1TQLxgKdMeTjDRU5GYxiGNkjUbSFFbM41A/wflT3xwMC6JUBA==" saltValue="E95l0uMiKnsRfFnfM9Vj+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dlG1VGpDlhmp/CpujabKx1aLWYIpTMtWp2rqpDUtduX7PDrcfUGq6TKko5SivbLIa2hOtD0UJwNG8oPV5ClLlg==" saltValue="R263Wt52X9OGhhYzJDQviQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4966,79 +4916,75 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="54.5" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="40.5" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="27" customWidth="1"/>
-    <col min="12" max="12" width="64.83203125" customWidth="1"/>
-    <col min="13" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="54.5" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="40.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="27" customWidth="1"/>
+    <col min="11" max="11" width="64.83203125" customWidth="1"/>
+    <col min="12" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="H1" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J2" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I2" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5046,7 +4992,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Private data" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" sqref="K1:K1002" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Private data" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" sqref="J1:J1002" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5058,9 +5004,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5070,394 +5018,386 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>87</v>
+      <c r="A20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8c2V3aKUuwLo6Wg9ODlPSWx7VCLjubS94Nxj8Xfx31DxXoQg8SXriTzYWZU8s8JvO9XSvSvndWYiDEksSLmCPQ==" saltValue="whsK0JIxIuClElcadbAp3g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="j+agHRtZZEgB1BvaTCdP4tD+WmFeT/qF0v0Fc8ItrFSFw9xB95qgqrmv+inbwzQlwZq1NFE4DfdkJhhjxKXDYQ==" saltValue="YeDTTolsbsA6UX5sksIeTg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -5465,10 +5405,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5476,79 +5416,71 @@
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="86.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="151.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="7.5" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" customWidth="1"/>
-    <col min="14" max="14" width="6.5" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="151.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.5" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="6.5" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>65</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C2" s="26"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C4" s="26"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PROJECT" prompt="This title will be diplayed on the EVA study page for your project" sqref="D2:D4" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="INSDC accession" prompt="Please provide the INSDC accession of the reference assembly/sequence used" sqref="F1:F1004" xr:uid="{00000000-0002-0000-0500-000001000000}">
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="INSDC accession" prompt="Please provide the INSDC accession of the reference assembly/sequence used" sqref="E1:E1004" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5557,16 +5489,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Project sheet" prompt="Must be the same project title from the title provided in the PROJECT SHEET" xr:uid="{00000000-0002-0000-0500-000003000000}">
-          <x14:formula1>
-            <xm:f>Project!$A$2</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>D1 D5:D1004</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000004000000}">
           <x14:formula1>
             <xm:f>CVs!$D$3:$D$9</xm:f>
@@ -5574,16 +5497,16 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E1:E1004</xm:sqref>
+          <xm:sqref>D1:D1004</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="New platform inserted" error="Are you sure the platform entered is correct?" promptTitle="Platform listing" prompt="Please select from the available list of platforms._x000a_If your platform is not present, please enter it as a new entry and confirm warning message" xr:uid="{00000000-0002-0000-0500-000005000000}">
           <x14:formula1>
-            <xm:f>'Analysis HELP'!$A$21:$A$72</xm:f>
+            <xm:f>'Analysis HELP'!$A$20:$A$71</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G1:G1004</xm:sqref>
+          <xm:sqref>F1:F1004</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5607,426 +5530,426 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B14" s="32"/>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B18" s="32"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B21" s="32"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B27" s="32"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B31" s="32"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B42" s="32"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B53" s="32"/>
     </row>
     <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="33" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B54" s="32"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B55" s="32"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -6041,7 +5964,7 @@
   <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6054,16 +5977,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="67"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="70" t="s">
-        <v>236</v>
+      <c r="A1" s="59"/>
+      <c r="C1" s="61" t="s">
+        <v>231</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>545</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>237</v>
+        <v>534</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>232</v>
       </c>
       <c r="F1" s="39"/>
       <c r="G1" s="40"/>
@@ -6107,198 +6029,198 @@
       <c r="AS1" s="43"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="68"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63" t="s">
+      <c r="A2" s="60"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="76"/>
+      <c r="AF2" s="76"/>
+      <c r="AG2" s="76"/>
+      <c r="AH2" s="76"/>
+      <c r="AI2" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ2" s="76"/>
+      <c r="AK2" s="76"/>
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="76"/>
+      <c r="AN2" s="76"/>
+      <c r="AO2" s="76"/>
+      <c r="AP2" s="76"/>
+      <c r="AQ2" s="76"/>
+      <c r="AR2" s="76"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="M3" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="62" t="s">
+      <c r="N3" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q3" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="S3" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62" t="s">
+      <c r="T3" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="U3" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="V3" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="W3" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="X3" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62" t="s">
+      <c r="Y3" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z3" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA3" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="62" t="s">
+      <c r="AB3" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC3" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD3" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE3" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF3" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG3" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH3" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI3" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ3" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="AK3" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>238</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="L3" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="M3" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="N3" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="O3" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="P3" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q3" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="R3" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="S3" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="T3" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="U3" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="V3" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="W3" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="X3" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="Y3" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="Z3" s="51" t="s">
-        <v>192</v>
-      </c>
-      <c r="AA3" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="AB3" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC3" s="47" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD3" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="AE3" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="AF3" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="AG3" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="AH3" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="AI3" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="AJ3" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="AK3" s="47" t="s">
-        <v>215</v>
-      </c>
       <c r="AL3" s="47" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AM3" s="47" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AN3" s="47" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AO3" s="47" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="AP3" s="47" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AQ3" s="47" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AR3" s="48" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AS3" s="52" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
@@ -6384,9 +6306,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6396,46 +6320,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="B4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8BWC8IcCh0oOImi6uJxkPf7THeVopfH3/UrpKnXK3baWYoESjyFXKEantxfvQWyCyfPwcyZ2QAYZwXSjJGwBHQ==" saltValue="0YcUWeoaM0DOc9w3C1Xe8g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ocmDvhTzY/TFrKeNd7NmJBzSBqU8yfYBCOiNI3pVL1HhRS2hH1UkFYM+XX3ywbQQcKpGjs4wYfNTsKujcRB5ag==" saltValue="lEqIHQcEiDEhtF5RAixf9g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
EVA-3581 Add option to see all errors of all categories for a sample (#41)
* add option to see all errors of all categories for a sample
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E726AD75-BC0A-734A-9759-1F7F3297F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE5AD1-A7DC-C143-BC36-7E1018F23EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35060" windowHeight="15300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="14800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -625,7 +625,7 @@
     <t>Template Basic Details</t>
   </si>
   <si>
-    <t>Sample Name</t>
+    <t>BioSample Name</t>
   </si>
   <si>
     <t>Unique sample identifier (e.g. st-ssff31)</t>
@@ -2193,13 +2193,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2214,7 +2241,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2257,6 +2290,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2310,43 +2346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2622,211 +2621,206 @@
     <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+    <row r="1" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" s="13" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="100" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="63"/>
-    </row>
-    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="MU1Ou8RkXCF2skpaTyap/rRlZ+lXNAvg7/CyPYvfUYxtHCfavXm69adfvvk8zyvIy5h/lXQdbiRBEwTzoTRiLA==" saltValue="3N3jbQAkrMCjyhvDt9mNXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -2835,6 +2829,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2846,7 +2845,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2856,10 +2855,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2906,25 +2905,25 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="36" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="36" t="s">
         <v>65</v>
       </c>
       <c r="E2" t="s">
@@ -2944,7 +2943,7 @@
       <c r="E3" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="61"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3392,7 +3391,7 @@
       <c r="B54" t="s">
         <v>313</v>
       </c>
-      <c r="E54" s="36"/>
+      <c r="E54" s="48"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
@@ -4541,7 +4540,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4555,31 +4554,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="22"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="C3" s="22"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4602,15 +4601,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="35" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
@@ -4618,7 +4617,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
@@ -4626,15 +4625,15 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="38" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
@@ -4714,10 +4713,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4732,9 +4731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4747,53 +4744,53 @@
     <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="9" width="40.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="28" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="39" customWidth="1"/>
     <col min="11" max="11" width="64.83203125" customWidth="1"/>
     <col min="12" max="13" width="6" customWidth="1"/>
     <col min="14" max="14" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="41" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4828,15 +4825,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="35" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
@@ -4844,7 +4841,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>62</v>
       </c>
       <c r="B3" t="s">
@@ -4852,7 +4849,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="s">
@@ -4860,7 +4857,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B5" t="s">
@@ -4868,7 +4865,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B6" t="s">
@@ -4876,7 +4873,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="74" t="s">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
       <c r="B7" t="s">
@@ -4956,7 +4953,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="36" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5218,7 +5215,10 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="DFETNWEFhDB9oWAe2KH3luSenDfafMszSC6Iy77AxfN5YtGJBx5U3QGkFDVXjdaoQmbaXUssrevKxTQwduXhpQ==" saltValue="n8f/udOcIHSKNrU1sFfIDA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0400-000000000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5229,9 +5229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5250,73 +5248,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="32" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="27"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="27"/>
+      <c r="C4" s="38"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="INSDC accession" prompt="Please provide the INSDC accession of the reference assembly/sequence used" sqref="E1:E1001 F2:F1001" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="INSDC accession" prompt="Please provide the INSDC accession of the reference assembly/sequence used" sqref="E1 E2:F1001" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reference file path" prompt="The path to the reference in fasta format that was used to create the VCF. (This is a local path)" sqref="F1" xr:uid="{7B43CC07-F741-8F43-A1ED-15DFE83C258F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reference file path" prompt="The path to the reference in fasta format that was used to create the VCF. (This is a local path)" sqref="F1" xr:uid="{00000000-0002-0000-0500-000001000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>
             <xm:f>CVs!$D$3:$D$9</xm:f>
           </x14:formula1>
@@ -5325,7 +5326,7 @@
           </x14:formula2>
           <xm:sqref>D1:D1001</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="New platform inserted" error="Are you sure the platform entered is correct?" promptTitle="Platform listing" prompt="Please select from the available list of platforms._x000a_If your platform is not present, please enter it as a new entry and confirm warning message" xr:uid="{00000000-0002-0000-0500-000002000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="New platform inserted" error="Are you sure the platform entered is correct?" promptTitle="Platform listing" prompt="Please select from the available list of platforms._x000a_If your platform is not present, please enter it as a new entry and confirm warning message" xr:uid="{00000000-0002-0000-0500-000003000000}">
           <x14:formula1>
             <xm:f>'Analysis HELP'!$A$21:$A$72</xm:f>
           </x14:formula1>
@@ -5345,7 +5346,7 @@
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5355,68 +5356,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="44" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="45" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="44" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="44" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="44" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="47" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="44" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5424,7 +5425,7 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="44" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5432,7 +5433,7 @@
       <c r="A11" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="44" t="s">
         <v>154</v>
       </c>
     </row>
@@ -5440,7 +5441,7 @@
       <c r="A12" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="44" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5448,29 +5449,29 @@
       <c r="A13" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="44" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="44"/>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="49" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="44" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5478,21 +5479,21 @@
       <c r="A17" t="s">
         <v>164</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="44" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="B18" s="32"/>
+      <c r="B18" s="44"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="44" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5500,21 +5501,21 @@
       <c r="A20" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="44" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="44"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>172</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="44" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5522,7 +5523,7 @@
       <c r="A23" t="s">
         <v>174</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="44" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5530,7 +5531,7 @@
       <c r="A24" t="s">
         <v>176</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="44" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5538,7 +5539,7 @@
       <c r="A25" t="s">
         <v>178</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="44" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5546,21 +5547,21 @@
       <c r="A26" t="s">
         <v>180</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="44" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="44"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>183</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="44" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5568,7 +5569,7 @@
       <c r="A29" t="s">
         <v>185</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="44" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5576,21 +5577,21 @@
       <c r="A30" t="s">
         <v>187</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="44" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="44"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="44" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5598,7 +5599,7 @@
       <c r="A33" t="s">
         <v>192</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="44" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5606,7 +5607,7 @@
       <c r="A34" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="44" t="s">
         <v>195</v>
       </c>
     </row>
@@ -5614,7 +5615,7 @@
       <c r="A35" t="s">
         <v>196</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="44" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5622,7 +5623,7 @@
       <c r="A36" t="s">
         <v>198</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="44" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5630,7 +5631,7 @@
       <c r="A37" t="s">
         <v>200</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="44" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5638,7 +5639,7 @@
       <c r="A38" t="s">
         <v>202</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="44" t="s">
         <v>203</v>
       </c>
     </row>
@@ -5646,7 +5647,7 @@
       <c r="A39" t="s">
         <v>204</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="44" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5654,7 +5655,7 @@
       <c r="A40" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="44" t="s">
         <v>207</v>
       </c>
     </row>
@@ -5662,21 +5663,21 @@
       <c r="A41" t="s">
         <v>208</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="49" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="44"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>211</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="44" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5684,7 +5685,7 @@
       <c r="A44" t="s">
         <v>213</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="44" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5692,7 +5693,7 @@
       <c r="A45" t="s">
         <v>215</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="44" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5700,7 +5701,7 @@
       <c r="A46" t="s">
         <v>217</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="44" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5708,7 +5709,7 @@
       <c r="A47" t="s">
         <v>219</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="44" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5716,7 +5717,7 @@
       <c r="A48" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="44" t="s">
         <v>222</v>
       </c>
     </row>
@@ -5724,7 +5725,7 @@
       <c r="A49" t="s">
         <v>223</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="44" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5732,7 +5733,7 @@
       <c r="A50" t="s">
         <v>225</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="44" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5740,7 +5741,7 @@
       <c r="A51" t="s">
         <v>227</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="44" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5748,38 +5749,38 @@
       <c r="A52" t="s">
         <v>229</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="44" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="B53" s="32"/>
+      <c r="B53" s="44"/>
     </row>
     <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B54" s="32"/>
+      <c r="B54" s="44"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="B55" s="32"/>
+      <c r="B55" s="44"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>234</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="44" t="s">
         <v>235</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IrtVTf7xUCmZBNRcjFMvaCyEJlvTB6oNqXh6XCTcGZac6l0HOs2PvYrIVUVf+JnmYqRLN7+7d4uhcaWbDdElXg==" saltValue="Kwd+oWgMyKFzDZZ5ZDzrwQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E50B" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -5790,7 +5791,7 @@
   <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5803,266 +5804,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="39"/>
-      <c r="C1" s="40" t="s">
+      <c r="A1" s="51"/>
+      <c r="C1" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="46"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="56"/>
+      <c r="AP1" s="56"/>
+      <c r="AQ1" s="56"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="58"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="47"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="73" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73" t="s">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="71" t="s">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71" t="s">
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="71"/>
-      <c r="AI2" s="71" t="s">
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AJ2" s="71"/>
-      <c r="AK2" s="71"/>
-      <c r="AL2" s="71"/>
-      <c r="AM2" s="71"/>
-      <c r="AN2" s="71"/>
-      <c r="AO2" s="71"/>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="51" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="M3" s="54" t="s">
+      <c r="M3" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="65" t="s">
         <v>167</v>
       </c>
-      <c r="O3" s="55" t="s">
+      <c r="O3" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="65" t="s">
         <v>240</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="Q3" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="R3" s="53" t="s">
+      <c r="R3" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="S3" s="65" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="53" t="s">
+      <c r="T3" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="U3" s="54" t="s">
+      <c r="U3" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="V3" s="56" t="s">
+      <c r="V3" s="68" t="s">
         <v>183</v>
       </c>
-      <c r="W3" s="53" t="s">
+      <c r="W3" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="X3" s="54" t="s">
+      <c r="X3" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="Y3" s="56" t="s">
+      <c r="Y3" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="Z3" s="57" t="s">
+      <c r="Z3" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="AA3" s="53" t="s">
+      <c r="AA3" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="AB3" s="53" t="s">
+      <c r="AB3" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="AC3" s="53" t="s">
+      <c r="AC3" s="65" t="s">
         <v>198</v>
       </c>
-      <c r="AD3" s="53" t="s">
+      <c r="AD3" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="AE3" s="53" t="s">
+      <c r="AE3" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="AF3" s="53" t="s">
+      <c r="AF3" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="AG3" s="53" t="s">
+      <c r="AG3" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="AH3" s="54" t="s">
+      <c r="AH3" s="66" t="s">
         <v>208</v>
       </c>
-      <c r="AI3" s="56" t="s">
+      <c r="AI3" s="68" t="s">
         <v>211</v>
       </c>
-      <c r="AJ3" s="53" t="s">
+      <c r="AJ3" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="AK3" s="53" t="s">
+      <c r="AK3" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="AL3" s="53" t="s">
+      <c r="AL3" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="AM3" s="53" t="s">
+      <c r="AM3" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="AN3" s="53" t="s">
+      <c r="AN3" s="65" t="s">
         <v>221</v>
       </c>
-      <c r="AO3" s="53" t="s">
+      <c r="AO3" s="65" t="s">
         <v>223</v>
       </c>
-      <c r="AP3" s="53" t="s">
+      <c r="AP3" s="65" t="s">
         <v>225</v>
       </c>
-      <c r="AQ3" s="53" t="s">
+      <c r="AQ3" s="65" t="s">
         <v>227</v>
       </c>
-      <c r="AR3" s="54" t="s">
+      <c r="AR3" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="AS3" s="58" t="s">
+      <c r="AS3" s="70" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L4" s="59"/>
-      <c r="X4" s="28"/>
+      <c r="L4" s="71"/>
+      <c r="X4" s="39"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L5" s="59"/>
-      <c r="X5" s="28"/>
+      <c r="L5" s="71"/>
+      <c r="X5" s="39"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L6" s="59"/>
-      <c r="X6" s="28"/>
+      <c r="L6" s="71"/>
+      <c r="X6" s="39"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L7" s="59"/>
+      <c r="L7" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6154,15 +6155,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="35" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>62</v>
       </c>
       <c r="B2" t="s">
@@ -6170,7 +6171,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>242</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Add casting as list, date and boolean when converting metadata to json
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE5AD1-A7DC-C143-BC36-7E1018F23EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EAB81C-1FDA-3B4B-9ABF-BF59741EEA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="14800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35840" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -304,24 +304,12 @@
     <t>Publication(s) related to the project, given in DB:ID form (e.g. PubMed:23128226, PubMed:223445)</t>
   </si>
   <si>
-    <t>Parent Project(s)</t>
-  </si>
-  <si>
-    <t>Accession OR Alias of all parent project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
-  </si>
-  <si>
     <t>Child Project(s)</t>
   </si>
   <si>
-    <t>Accession OR Alias of all child project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
-  </si>
-  <si>
     <t>Peert Project(s)</t>
   </si>
   <si>
-    <t>Accession OR Alias of all peer project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
-  </si>
-  <si>
     <t>Link(s)</t>
   </si>
   <si>
@@ -1802,6 +1790,18 @@
   </si>
   <si>
     <t>restricted access</t>
+  </si>
+  <si>
+    <t>Parent Project</t>
+  </si>
+  <si>
+    <t>Accession of a single parent project of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
+  </si>
+  <si>
+    <t>Accession of all child project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
+  </si>
+  <si>
+    <t>Accession of all peer project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
   </si>
 </sst>
 </file>
@@ -2195,38 +2195,11 @@
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2241,13 +2214,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2345,6 +2312,39 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2611,7 +2611,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2621,206 +2621,211 @@
     <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="B4" s="69"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="80" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="66"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="100" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="63"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="63"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="63"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="B22" s="63"/>
+    </row>
+    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="MU1Ou8RkXCF2skpaTyap/rRlZ+lXNAvg7/CyPYvfUYxtHCfavXm69adfvvk8zyvIy5h/lXQdbiRBEwTzoTRiLA==" saltValue="3N3jbQAkrMCjyhvDt9mNXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -2829,11 +2834,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2855,11 +2855,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>242</v>
+      <c r="A1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2905,1627 +2905,1627 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="72" t="s">
+    <row r="1" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>71</v>
+      <c r="E1" s="25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>65</v>
+      <c r="A2" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="73"/>
+        <v>86</v>
+      </c>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E35" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E42" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E43" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E44" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E47" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E48" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E49" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E52" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>313</v>
-      </c>
-      <c r="E54" s="48"/>
+        <v>309</v>
+      </c>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -4554,31 +4554,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="33"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="C3" s="33"/>
-      <c r="E3" s="34"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4591,7 +4591,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4601,15 +4601,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
@@ -4617,7 +4617,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
@@ -4625,15 +4625,15 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="27" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
@@ -4650,78 +4650,78 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>537</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>58</v>
+      <c r="A15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dlG1VGpDlhmp/CpujabKx1aLWYIpTMtWp2rqpDUtduX7PDrcfUGq6TKko5SivbLIa2hOtD0UJwNG8oPV5ClLlg==" saltValue="R263Wt52X9OGhhYzJDQviQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UWfECU9Bs7KCbWVgSD7qb4y5kuVNnaEUFYFircSXE2o/i+Hwf+w4bzwcMZaywIbI08zp/PtCvxtri5q/A1hN7A==" saltValue="W1qyJUouiHZldYwW/oVbKA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4731,7 +4731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4744,54 +4746,54 @@
     <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="9" width="40.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="39" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="28" customWidth="1"/>
     <col min="11" max="11" width="64.83203125" customWidth="1"/>
     <col min="12" max="13" width="6" customWidth="1"/>
     <col min="14" max="14" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="L1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="M1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="N1" s="30" t="s">
         <v>53</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4825,391 +4827,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
-        <v>88</v>
+      <c r="A20" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -5248,58 +5250,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="30" t="s">
+      <c r="A1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="H1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="I1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="J1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="K1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="L1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="M1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="32" t="s">
-        <v>86</v>
+      <c r="N1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="38"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="38"/>
+      <c r="C4" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5356,427 +5358,427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="B5" s="33" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B6" s="33" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="44" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="B8" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="44" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="B9" s="33" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="44" t="s">
-        <v>152</v>
+      <c r="B10" s="33" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="33"/>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="44" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+      <c r="B16" s="33" t="s">
         <v>159</v>
-      </c>
-      <c r="B14" s="44"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="44"/>
+      <c r="A18" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="33"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>168</v>
+        <v>163</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="44"/>
+      <c r="A21" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="33"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>177</v>
+        <v>172</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>179</v>
+        <v>174</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>180</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" s="44"/>
+      <c r="A27" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>185</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>187</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>188</v>
+        <v>183</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="B31" s="44"/>
+      <c r="A31" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="33"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>193</v>
+        <v>188</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>199</v>
+        <v>194</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>203</v>
+        <v>198</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>205</v>
+        <v>200</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>206</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>207</v>
+        <v>202</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>208</v>
-      </c>
-      <c r="B41" s="49" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="44"/>
+      <c r="A42" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="33"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>213</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>215</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>216</v>
+        <v>211</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>217</v>
-      </c>
-      <c r="B46" s="44" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>219</v>
-      </c>
-      <c r="B47" s="44" t="s">
-        <v>220</v>
+        <v>215</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>221</v>
-      </c>
-      <c r="B48" s="44" t="s">
-        <v>222</v>
+        <v>217</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>223</v>
-      </c>
-      <c r="B49" s="44" t="s">
-        <v>224</v>
+        <v>219</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>225</v>
-      </c>
-      <c r="B50" s="44" t="s">
-        <v>226</v>
+        <v>221</v>
+      </c>
+      <c r="B50" s="33" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>227</v>
-      </c>
-      <c r="B51" s="44" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>225</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="33"/>
+    </row>
+    <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" s="33"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="B52" s="44" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="B53" s="44"/>
-    </row>
-    <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="B54" s="44"/>
-    </row>
-    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="B55" s="44"/>
+      <c r="B55" s="33"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>234</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -5804,266 +5806,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="51"/>
-      <c r="C1" s="52" t="s">
+      <c r="A1" s="40"/>
+      <c r="C1" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="47"/>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A2" s="48"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ2" s="71"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="72"/>
+      <c r="E3" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="L3" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="M3" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" s="54" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AQ1" s="56"/>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="58"/>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="63" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="64" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="L3" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="M3" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="N3" s="65" t="s">
-        <v>167</v>
-      </c>
-      <c r="O3" s="67" t="s">
-        <v>169</v>
-      </c>
-      <c r="P3" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q3" s="68" t="s">
+      <c r="Q3" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="R3" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="S3" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="R3" s="65" t="s">
+      <c r="T3" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="S3" s="65" t="s">
+      <c r="U3" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="65" t="s">
-        <v>178</v>
-      </c>
-      <c r="U3" s="66" t="s">
-        <v>180</v>
-      </c>
-      <c r="V3" s="68" t="s">
+      <c r="V3" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="W3" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="X3" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="W3" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="X3" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="Y3" s="68" t="s">
+      <c r="Y3" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z3" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA3" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="Z3" s="69" t="s">
+      <c r="AB3" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="AA3" s="65" t="s">
+      <c r="AC3" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="AB3" s="65" t="s">
+      <c r="AD3" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="AC3" s="65" t="s">
+      <c r="AE3" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="AD3" s="65" t="s">
+      <c r="AF3" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="AE3" s="65" t="s">
+      <c r="AG3" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="AF3" s="65" t="s">
+      <c r="AH3" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="AG3" s="65" t="s">
-        <v>206</v>
-      </c>
-      <c r="AH3" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="AI3" s="68" t="s">
+      <c r="AI3" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ3" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="AK3" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="AJ3" s="65" t="s">
+      <c r="AL3" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="AK3" s="65" t="s">
+      <c r="AM3" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AN3" s="54" t="s">
         <v>217</v>
       </c>
-      <c r="AM3" s="65" t="s">
+      <c r="AO3" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="AN3" s="65" t="s">
+      <c r="AP3" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="AO3" s="65" t="s">
+      <c r="AQ3" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="AP3" s="65" t="s">
+      <c r="AR3" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="AQ3" s="65" t="s">
+      <c r="AS3" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="AR3" s="66" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS3" s="70" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L4" s="71"/>
-      <c r="X4" s="39"/>
+      <c r="L4" s="60"/>
+      <c r="X4" s="28"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L5" s="71"/>
-      <c r="X5" s="39"/>
+      <c r="L5" s="60"/>
+      <c r="X5" s="28"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L6" s="71"/>
-      <c r="X6" s="39"/>
+      <c r="L6" s="60"/>
+      <c r="X6" s="28"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L7" s="71"/>
+      <c r="L7" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6155,27 +6157,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>62</v>
+      <c r="A2" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>242</v>
+      <c r="A3" s="25" t="s">
+        <v>238</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Transcriptomics and move Platform CV to the CVs tab
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EAB81C-1FDA-3B4B-9ABF-BF59741EEA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F839C2-407A-9A49-9C04-C070176A48DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="541">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Experiment Type</t>
   </si>
   <si>
-    <t>Choose 1 of the following "Whole genome sequencing", "Exome sequencing"', "Genotyping by array", "Curation","Whole transcriptome sequencing","Genotyping by sequencing","Target sequencing"</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -379,15 +376,9 @@
     <t>Reference Fasta Path</t>
   </si>
   <si>
-    <t>The path to the reference in fasta format that was used to create the VCF. (This is a local path)</t>
-  </si>
-  <si>
     <t>Platform</t>
   </si>
   <si>
-    <t>Enter the platform(s) used in the analysis separated by commas. See Platform CV below. If a platform was used which is not listed, please contact eva-helpdesk@ebi.ac.uk</t>
-  </si>
-  <si>
     <t>Software</t>
   </si>
   <si>
@@ -430,12 +421,6 @@
     <t>Run Accession(s)</t>
   </si>
   <si>
-    <t>Associated ENA run accession(s) if applicable (e.g. SRR576651, SRR576652)</t>
-  </si>
-  <si>
-    <t>Platform CV</t>
-  </si>
-  <si>
     <t>454 GS</t>
   </si>
   <si>
@@ -1802,6 +1787,21 @@
   </si>
   <si>
     <t>Accession of all peer project(s) of this project (NCBI, ENA, EVA all share the same project accession space so no database distinction is necessary) (e.g. PRJEB4019)</t>
+  </si>
+  <si>
+    <t>Comma separated list of associated ENA run accession(s) if applicable (e.g. SRR576651, SRR576652)</t>
+  </si>
+  <si>
+    <t>The path to the reference in fasta format that was used to create the VCF. (This is a local path on your file system)</t>
+  </si>
+  <si>
+    <t>Choose Experiment type based on the controled vocabulary in the CVs tab of this spreadsheet. If an experiment type is not listed, please contact eva-helpdesk@ebi.ac.uk</t>
+  </si>
+  <si>
+    <t>Transcriptomics</t>
+  </si>
+  <si>
+    <t>Enter the platform(s) used in the analysis separated by commas. See Platform CV in the CVs tab of this spreadsheet. You can use other platforms if needed</t>
   </si>
 </sst>
 </file>
@@ -2313,17 +2313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2336,6 +2327,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2611,7 +2611,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2622,8 +2622,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2632,10 +2632,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2644,10 +2644,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2656,10 +2656,10 @@
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="69"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2668,10 +2668,10 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="70"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2704,8 +2704,8 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2714,10 +2714,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2726,8 +2726,8 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2736,10 +2736,10 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="70"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -2791,28 +2791,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="68"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="68"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="68"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="68"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
@@ -2821,11 +2821,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="MU1Ou8RkXCF2skpaTyap/rRlZ+lXNAvg7/CyPYvfUYxtHCfavXm69adfvvk8zyvIy5h/lXQdbiRBEwTzoTRiLA==" saltValue="3N3jbQAkrMCjyhvDt9mNXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -2834,6 +2829,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2859,7 +2859,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2894,7 +2894,7 @@
   <dimension ref="A1:F281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2907,1629 +2907,1633 @@
   <sheetData>
     <row r="1" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>67</v>
-      </c>
+      <c r="E1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
-        <v>85</v>
+      <c r="E2" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B9" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>258</v>
+      </c>
+      <c r="D10" t="s">
+        <v>539</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E43" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E45" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E46" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E47" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E48" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E49" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E50" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E51" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>308</v>
+        <v>303</v>
+      </c>
+      <c r="E53" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>309</v>
-      </c>
-      <c r="E54" s="37"/>
+        <v>304</v>
+      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>310</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="E55" s="37"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YpxYS3YarbEcU6tWwuRMfCKS/4VgrVauR8PgXRA9n+H1kMj1rZpzdUBeRpn2V18P1MjYz2grSS8/2LmiS55opA==" saltValue="fjdpxiVJrkefuObTwVSAQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2UEJdRlxuFs2VTiNtFVX1W9jQghsYU2f6R22TmIfBHdHwTna1Bwm7rHER5tKHVeKX0/RFVWDOxwgcYsugE1mRQ==" saltValue="quPywOOGgd0riLFsHmAUsw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4650,10 +4654,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B7" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4661,7 +4665,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4669,7 +4673,7 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4769,7 +4773,7 @@
         <v>39</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>41</v>
@@ -4814,10 +4818,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4863,79 +4867,79 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -4943,279 +4947,22 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>134</v>
-      </c>
+      <c r="A20" s="25"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DFETNWEFhDB9oWAe2KH3luSenDfafMszSC6Iy77AxfN5YtGJBx5U3QGkFDVXjdaoQmbaXUssrevKxTQwduXhpQ==" saltValue="n8f/udOcIHSKNrU1sFfIDA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="EOI/+Bpbq0+4Ug6fJ9OKBUxk79nUHv6LMg2HlCWxdcaFtqYyK2dhLSN1OTLoGQf25hC4c4G8tnlSPRQFy7LM/g==" saltValue="nLbZfwj5L+3Zo1Z30qWMrw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0</formula1>
@@ -5231,7 +4978,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5263,37 +5012,37 @@
         <v>61</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F1" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>67</v>
-      </c>
       <c r="H1" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>43</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -5318,7 +5067,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>
             <xm:f>CVs!$D$3:$D$9</xm:f>
@@ -5335,7 +5084,13 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G1:G1001</xm:sqref>
+          <xm:sqref>G1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="New platform inserted" error="Are you sure the platform entered is correct?" promptTitle="Platform listing" prompt="Please select from the available list of platforms._x000a_If your platform is not present, please enter it as a new entry and confirm warning message" xr:uid="{35E0B72D-C7D3-3B40-BB08-561EDA1B7B87}">
+          <x14:formula1>
+            <xm:f>CVs!$E$3:$E$53</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1001</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5370,57 +5125,57 @@
         <v>58</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5428,357 +5183,357 @@
         <v>34</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B18" s="33"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B21" s="33"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B31" s="33"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="37" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B42" s="33"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="37" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B53" s="33"/>
     </row>
     <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="34" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B54" s="33"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B55" s="33"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5808,13 +5563,13 @@
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="40"/>
       <c r="C1" s="41" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F1" s="43"/>
       <c r="G1" s="44"/>
@@ -5863,7 +5618,7 @@
       <c r="C2" s="49"/>
       <c r="D2" s="72"/>
       <c r="E2" s="71" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F2" s="71"/>
       <c r="G2" s="71"/>
@@ -5871,29 +5626,29 @@
       <c r="I2" s="71"/>
       <c r="J2" s="71"/>
       <c r="K2" s="73" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="L2" s="73"/>
       <c r="M2" s="73"/>
       <c r="N2" s="73" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O2" s="73"/>
       <c r="P2" s="73"/>
       <c r="Q2" s="71" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="R2" s="71"/>
       <c r="S2" s="71"/>
       <c r="T2" s="71"/>
       <c r="U2" s="71"/>
       <c r="V2" s="71" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="W2" s="71"/>
       <c r="X2" s="71"/>
       <c r="Y2" s="71" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Z2" s="71"/>
       <c r="AA2" s="71"/>
@@ -5905,7 +5660,7 @@
       <c r="AG2" s="71"/>
       <c r="AH2" s="71"/>
       <c r="AI2" s="71" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AJ2" s="71"/>
       <c r="AK2" s="71"/>
@@ -5922,134 +5677,134 @@
         <v>58</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D3" s="72"/>
       <c r="E3" s="52" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F3" s="53" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G3" s="54" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="54" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I3" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="K3" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="L3" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="K3" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" s="53" t="s">
+      <c r="M3" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="N3" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="M3" s="55" t="s">
+      <c r="O3" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="P3" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q3" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="R3" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="P3" s="54" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q3" s="57" t="s">
-        <v>168</v>
-      </c>
-      <c r="R3" s="54" t="s">
-        <v>170</v>
-      </c>
       <c r="S3" s="54" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="T3" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="V3" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="W3" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="V3" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="W3" s="54" t="s">
+      <c r="X3" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y3" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="X3" s="55" t="s">
+      <c r="Z3" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="Y3" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="Z3" s="58" t="s">
-        <v>188</v>
-      </c>
       <c r="AA3" s="54" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="AB3" s="54" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="AC3" s="54" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AD3" s="54" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AE3" s="54" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="AF3" s="54" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AG3" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH3" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI3" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="AH3" s="55" t="s">
+      <c r="AJ3" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="AI3" s="57" t="s">
-        <v>207</v>
-      </c>
-      <c r="AJ3" s="54" t="s">
-        <v>209</v>
-      </c>
       <c r="AK3" s="54" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AL3" s="54" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AM3" s="54" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AN3" s="54" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AO3" s="54" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AP3" s="54" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AQ3" s="54" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="AR3" s="55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AS3" s="59" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
@@ -6169,15 +5924,15 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sample help tab
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F839C2-407A-9A49-9C04-C070176A48DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDD7398-32CA-F54E-950A-A574934E4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="539">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -574,36 +574,15 @@
     <t>Alias of the analysis performed on this sample. Comma separated list allowable for multiple analyses</t>
   </si>
   <si>
-    <t>For each sample, please complete either the "Pre-registered sample(s)" OR "Novel sample(s)" sections</t>
-  </si>
-  <si>
     <t>Sample Accession</t>
   </si>
   <si>
-    <t>Accession of the sample (BioSamples, ENA or EGA)</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
-    <t>Sample ID used in the VCF file</t>
-  </si>
-  <si>
-    <t>Sampleset Accession</t>
-  </si>
-  <si>
-    <t>BioSamples sampleset accession if apporpriate</t>
-  </si>
-  <si>
     <t>Template Basic Details</t>
   </si>
   <si>
     <t>BioSample Name</t>
   </si>
   <si>
-    <t>Unique sample identifier (e.g. st-ssff31)</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -1802,6 +1781,21 @@
   </si>
   <si>
     <t>Enter the platform(s) used in the analysis separated by commas. See Platform CV in the CVs tab of this spreadsheet. You can use other platforms if needed</t>
+  </si>
+  <si>
+    <t>For each sample, please complete either  "Pre-registered sample(s)" OR "Novel sample(s)" sections</t>
+  </si>
+  <si>
+    <t>Analysis alias from Analysis tab associated with this sample. You can use comma separated list of alias if associated with multiple analysis.</t>
+  </si>
+  <si>
+    <t>Name of this sample as if appears in the VCF file</t>
+  </si>
+  <si>
+    <t>BioSample Accession of For Pre Existing sample. Only use for preregistered samples</t>
+  </si>
+  <si>
+    <t>Unique sample identifier which will be used as name in the Biosamples</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +1805,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1992,6 +1986,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2193,7 +2202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2265,7 +2274,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2306,15 +2314,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2328,15 +2344,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2346,6 +2353,16 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2622,8 +2639,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2632,10 +2649,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2644,10 +2661,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2656,10 +2673,10 @@
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="66"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2668,10 +2685,10 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2704,8 +2721,8 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2714,10 +2731,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="69"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2726,8 +2743,8 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2736,10 +2753,10 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="70"/>
+      <c r="B11" s="64"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -2791,28 +2808,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="68"/>
+      <c r="B19" s="61"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="68"/>
+      <c r="B20" s="61"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="68"/>
+      <c r="B21" s="61"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="68"/>
+      <c r="B22" s="61"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
@@ -2821,6 +2838,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="MU1Ou8RkXCF2skpaTyap/rRlZ+lXNAvg7/CyPYvfUYxtHCfavXm69adfvvk8zyvIy5h/lXQdbiRBEwTzoTRiLA==" saltValue="3N3jbQAkrMCjyhvDt9mNXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -2829,11 +2851,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2859,7 +2876,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2905,21 +2922,21 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>235</v>
-      </c>
-      <c r="D1" s="61" t="s">
+    <row r="1" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="59" t="s">
         <v>16</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>61</v>
@@ -2930,28 +2947,28 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E4" t="s">
         <v>81</v>
@@ -2959,13 +2976,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E5" t="s">
         <v>82</v>
@@ -2973,13 +2990,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -2987,13 +3004,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E7" t="s">
         <v>84</v>
@@ -3001,13 +3018,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E8" t="s">
         <v>85</v>
@@ -3015,13 +3032,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E9" t="s">
         <v>86</v>
@@ -3029,13 +3046,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="E10" t="s">
         <v>87</v>
@@ -3043,10 +3060,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E11" t="s">
         <v>88</v>
@@ -3054,10 +3071,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E12" t="s">
         <v>88</v>
@@ -3065,7 +3082,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="E13" t="s">
         <v>89</v>
@@ -3073,7 +3090,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E14" t="s">
         <v>90</v>
@@ -3081,7 +3098,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E15" t="s">
         <v>91</v>
@@ -3089,7 +3106,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E16" t="s">
         <v>92</v>
@@ -3097,7 +3114,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
@@ -3105,7 +3122,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E18" t="s">
         <v>94</v>
@@ -3113,7 +3130,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E19" t="s">
         <v>95</v>
@@ -3121,7 +3138,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E20" t="s">
         <v>96</v>
@@ -3129,7 +3146,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E21" t="s">
         <v>97</v>
@@ -3137,7 +3154,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E22" t="s">
         <v>98</v>
@@ -3145,7 +3162,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E23" t="s">
         <v>99</v>
@@ -3153,7 +3170,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E24" t="s">
         <v>100</v>
@@ -3161,7 +3178,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E25" t="s">
         <v>101</v>
@@ -3169,7 +3186,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E26" t="s">
         <v>102</v>
@@ -3177,7 +3194,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E27" t="s">
         <v>103</v>
@@ -3185,7 +3202,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E28" t="s">
         <v>104</v>
@@ -3193,7 +3210,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E29" t="s">
         <v>105</v>
@@ -3201,7 +3218,7 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E30" t="s">
         <v>106</v>
@@ -3209,7 +3226,7 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E31" t="s">
         <v>107</v>
@@ -3217,7 +3234,7 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E32" t="s">
         <v>108</v>
@@ -3225,7 +3242,7 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E33" t="s">
         <v>109</v>
@@ -3233,7 +3250,7 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E34" t="s">
         <v>110</v>
@@ -3241,7 +3258,7 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E35" t="s">
         <v>111</v>
@@ -3249,7 +3266,7 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E36" t="s">
         <v>112</v>
@@ -3257,7 +3274,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E37" t="s">
         <v>113</v>
@@ -3265,7 +3282,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E38" t="s">
         <v>114</v>
@@ -3273,7 +3290,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E39" t="s">
         <v>115</v>
@@ -3281,7 +3298,7 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E40" t="s">
         <v>116</v>
@@ -3289,7 +3306,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E41" t="s">
         <v>117</v>
@@ -3297,7 +3314,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E42" t="s">
         <v>118</v>
@@ -3305,7 +3322,7 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E43" t="s">
         <v>119</v>
@@ -3313,7 +3330,7 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E44" t="s">
         <v>120</v>
@@ -3321,7 +3338,7 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E45" t="s">
         <v>121</v>
@@ -3329,7 +3346,7 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E46" t="s">
         <v>122</v>
@@ -3337,7 +3354,7 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E47" t="s">
         <v>123</v>
@@ -3345,7 +3362,7 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E48" t="s">
         <v>124</v>
@@ -3353,7 +3370,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E49" t="s">
         <v>125</v>
@@ -3361,7 +3378,7 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E50" t="s">
         <v>126</v>
@@ -3369,7 +3386,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E51" t="s">
         <v>127</v>
@@ -3377,7 +3394,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E52" t="s">
         <v>128</v>
@@ -3385,7 +3402,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E53" t="s">
         <v>129</v>
@@ -3393,1143 +3410,1143 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>305</v>
-      </c>
-      <c r="E55" s="37"/>
+        <v>298</v>
+      </c>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -4654,10 +4671,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="B7" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4665,7 +4682,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4673,7 +4690,7 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4773,7 +4790,7 @@
         <v>39</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>41</v>
@@ -4867,7 +4884,7 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4883,7 +4900,7 @@
         <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4891,7 +4908,7 @@
         <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4955,7 +4972,7 @@
         <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -5100,10 +5117,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5112,7 +5129,7 @@
     <col min="2" max="2" width="212" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
@@ -5120,7 +5137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>58</v>
       </c>
@@ -5128,416 +5145,417 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="74" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="B6" s="33" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="33" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="B8" s="33" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B9" s="33" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B14" s="33"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B15" s="37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B16" s="33" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="33"/>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
-        <v>157</v>
+      <c r="A18" s="36" t="s">
+        <v>150</v>
       </c>
       <c r="B18" s="33"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
-        <v>162</v>
+      <c r="A21" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="B21" s="33"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>173</v>
+      <c r="A27" s="36" t="s">
+        <v>166</v>
       </c>
       <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="37" t="s">
-        <v>180</v>
+      <c r="A31" s="36" t="s">
+        <v>173</v>
       </c>
       <c r="B31" s="33"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>183</v>
+      <c r="A33" s="75" t="s">
+        <v>176</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>185</v>
+      <c r="A34" s="75" t="s">
+        <v>178</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>199</v>
-      </c>
-      <c r="B41" s="38" t="s">
-        <v>200</v>
+        <v>192</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="37" t="s">
-        <v>201</v>
+      <c r="A42" s="36" t="s">
+        <v>194</v>
       </c>
       <c r="B42" s="33"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="37" t="s">
-        <v>222</v>
+      <c r="A53" s="36" t="s">
+        <v>215</v>
       </c>
       <c r="B53" s="33"/>
     </row>
     <row r="54" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="34" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B54" s="33"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39" t="s">
-        <v>224</v>
+      <c r="A55" s="38" t="s">
+        <v>217</v>
       </c>
       <c r="B55" s="33"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="E50B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZdO7WY1ERAciVblJxucbhE4M4uXNQqLVnAhTlDcFHHWo+dAXp5qtg69TpFwdbpBXV3WibUWvINR5ivRIqoI4ow==" saltValue="d2mHMZHLmIEifj8uv4Rq6w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -5545,316 +5563,321 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="C1" s="41" t="s">
-        <v>227</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>228</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>229</v>
-      </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="46"/>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A1" s="39"/>
+      <c r="D1" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
       <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
-      <c r="AK1" s="45"/>
-      <c r="AL1" s="45"/>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="45"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
-      <c r="AR1" s="45"/>
-      <c r="AS1" s="47"/>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="73" t="s">
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="46"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A2" s="47"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="71" t="s">
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="69" t="s">
+        <v>166</v>
+      </c>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69"/>
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK2" s="69"/>
+      <c r="AL2" s="69"/>
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69"/>
+      <c r="AO2" s="69"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="69"/>
+      <c r="AS2" s="69"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A3" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="70"/>
+      <c r="F3" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="M3" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="O3" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="P3" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q3" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="R3" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="S3" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="T3" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="U3" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71" t="s">
+      <c r="V3" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="W3" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="X3" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y3" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z3" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA3" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB3" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC3" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="71"/>
-      <c r="AI2" s="71" t="s">
+      <c r="AD3" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE3" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF3" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG3" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH3" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI3" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ3" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="AK3" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="AL3" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="AM3" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="AJ2" s="71"/>
-      <c r="AK2" s="71"/>
-      <c r="AL2" s="71"/>
-      <c r="AM2" s="71"/>
-      <c r="AN2" s="71"/>
-      <c r="AO2" s="71"/>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="I3" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="K3" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="L3" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="M3" s="55" t="s">
-        <v>155</v>
-      </c>
-      <c r="N3" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="O3" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="P3" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q3" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="R3" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="S3" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="T3" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="U3" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="V3" s="57" t="s">
-        <v>174</v>
-      </c>
-      <c r="W3" s="54" t="s">
-        <v>176</v>
-      </c>
-      <c r="X3" s="55" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y3" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z3" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA3" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB3" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC3" s="54" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD3" s="54" t="s">
-        <v>191</v>
-      </c>
-      <c r="AE3" s="54" t="s">
-        <v>193</v>
-      </c>
-      <c r="AF3" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG3" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH3" s="55" t="s">
-        <v>199</v>
-      </c>
-      <c r="AI3" s="57" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ3" s="54" t="s">
-        <v>204</v>
-      </c>
-      <c r="AK3" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="AL3" s="54" t="s">
-        <v>208</v>
-      </c>
-      <c r="AM3" s="54" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN3" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="AO3" s="54" t="s">
-        <v>214</v>
-      </c>
-      <c r="AP3" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="AQ3" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="AR3" s="55" t="s">
-        <v>220</v>
-      </c>
-      <c r="AS3" s="59" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L4" s="60"/>
-      <c r="X4" s="28"/>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L5" s="60"/>
-      <c r="X5" s="28"/>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L6" s="60"/>
-      <c r="X6" s="28"/>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="L7" s="60"/>
+      <c r="AN3" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO3" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP3" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="AQ3" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="AR3" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS3" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="AT3" s="57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M4" s="58"/>
+      <c r="Y4" s="28"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M5" s="58"/>
+      <c r="Y5" s="28"/>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M6" s="58"/>
+      <c r="Y6" s="28"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M7" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AH2"/>
-    <mergeCell ref="AI2:AR2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AI2"/>
+    <mergeCell ref="AJ2:AS2"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:V2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1:A3" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="D1:E1 B2 E2 B4:B31 E4:E6 E8:E30 B32:B1003" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="E1:F1 B2:C2 F2 B4:C31 F4:F6 F8:F30 B32:C1003" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="Z1:Z3 X4:X6" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA3 Y4:Y6" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names Are used for new BioSample accession." sqref="E3" xr:uid="{00000000-0002-0000-0700-000003000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names Are used for new BioSample accession." sqref="F3" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample Name in VCF" prompt="These sample names must match those provided in the VCF file(s). They can be different from the sample name provided to new BioSamples  " sqref="B3" xr:uid="{00000000-0002-0000-0700-000004000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample Name in VCF" prompt="These sample names must match those provided in the VCF file(s). They can be different from the sample name provided to new BioSamples  " sqref="B3:C3" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="BioSample Accession" prompt="This column is used to provide pre-registered BioSample. Only one BioSample can be provided per cell" sqref="C3" xr:uid="{00000000-0002-0000-0700-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="BioSample Accession" prompt="This column is used to provide pre-registered BioSample. Only one BioSample can be provided per cell" sqref="D3" xr:uid="{00000000-0002-0000-0700-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5880,7 +5903,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AA1:AA3 Y4:Y6</xm:sqref>
+          <xm:sqref>AB1:AB3 Z4:Z6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0700-000008000000}">
           <x14:formula1>
@@ -5889,7 +5912,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>O1:O3 O7</xm:sqref>
+          <xm:sqref>P1:P3 P7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5924,15 +5947,15 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>